<commit_message>
Vince Added Test Case
</commit_message>
<xml_diff>
--- a/06 Software Testing/Test Template.xlsx
+++ b/06 Software Testing/Test Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\it601\IT601-2024\06 Software Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A166E5F4-84AD-446A-B3E0-D4D8A61C05AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1393708-D86B-43AE-9DE1-5C513CF6B8C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Case" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="104">
   <si>
     <t>Module Name</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>TC_001</t>
-  </si>
-  <si>
-    <t>Cyrill Endozo</t>
   </si>
   <si>
     <t>To check login functionality of Rogationist College Student Portal</t>
@@ -202,48 +199,6 @@
     <t>TC_011</t>
   </si>
   <si>
-    <t>TC_012</t>
-  </si>
-  <si>
-    <t>TC_013</t>
-  </si>
-  <si>
-    <t>TC_014</t>
-  </si>
-  <si>
-    <t>TC_015</t>
-  </si>
-  <si>
-    <t>TC_016</t>
-  </si>
-  <si>
-    <t>TC_017</t>
-  </si>
-  <si>
-    <t>TC_018</t>
-  </si>
-  <si>
-    <t>TC_019</t>
-  </si>
-  <si>
-    <t>TC_020</t>
-  </si>
-  <si>
-    <t>TC_021</t>
-  </si>
-  <si>
-    <t>TC_022</t>
-  </si>
-  <si>
-    <t>TC_023</t>
-  </si>
-  <si>
-    <t>TC_024</t>
-  </si>
-  <si>
-    <t>TC_025</t>
-  </si>
-  <si>
     <t>Bug_001</t>
   </si>
   <si>
@@ -290,6 +245,126 @@
   </si>
   <si>
     <t>03/25/2024</t>
+  </si>
+  <si>
+    <t>Check if the system denied your sign in attempt if you enter a wrong username and password.</t>
+  </si>
+  <si>
+    <t>Sarmiento Vince</t>
+  </si>
+  <si>
+    <t>Username: CT1234
+Password: ABCD123</t>
+  </si>
+  <si>
+    <t>Login unsuccessful</t>
+  </si>
+  <si>
+    <t>Check if the system accepet your log in attempt if you enter the following username and password</t>
+  </si>
+  <si>
+    <t>Check if the system denied your sign in attempt if you enter a correct username and wrong password.</t>
+  </si>
+  <si>
+    <t>Check if the system denied your sign in attempt if you enter a wrong username but correct password.</t>
+  </si>
+  <si>
+    <t>Username: CT221234
+Password: sarmiento#1221</t>
+  </si>
+  <si>
+    <t>When forgot password is click, user should be redirected to Recover Password Facility page.</t>
+  </si>
+  <si>
+    <t>user should be redirected to Recover Password Facility page</t>
+  </si>
+  <si>
+    <t>Redirecting to Recover Facilityt Page successful</t>
+  </si>
+  <si>
+    <t>Redirecting to facility page successful</t>
+  </si>
+  <si>
+    <t>When No account? Create One is click, user should redirect to members registration facility.</t>
+  </si>
+  <si>
+    <t>user should be redirected to Member Facility page.</t>
+  </si>
+  <si>
+    <t>1. Open the browser
+2. Launch Rogationist College Student Portal 
+3. Enter the username in username field
+4. Click on the Forgot Password.</t>
+  </si>
+  <si>
+    <t>1. Open the browser
+2. Launch Rogationist College Student Portal 
+3. Click on the No Account? Create One button.</t>
+  </si>
+  <si>
+    <t>Redirecting to Members Registration Facility page successful</t>
+  </si>
+  <si>
+    <t>Redirecting to Members Registration Facilityt Page successful.</t>
+  </si>
+  <si>
+    <t>Username: vincezander
+Password: sarmiento#1221</t>
+  </si>
+  <si>
+    <t>Username: vincezander
+Password: qwerty123</t>
+  </si>
+  <si>
+    <t>Check if the system automatically logged in even if the user did not enter username and password.</t>
+  </si>
+  <si>
+    <t>User name did not enter a username and password.</t>
+  </si>
+  <si>
+    <t>1. Open the browser
+2. Launch Rogationist College Student Portal
+3. Click on the Login button</t>
+  </si>
+  <si>
+    <t>Check if the system accepet your log in attempt if you only enter the password.</t>
+  </si>
+  <si>
+    <t>Username: none  Password: sarmiento#1221</t>
+  </si>
+  <si>
+    <t>1. Open the browser
+2. Launch Rogationist College Student Portal 
+3. Enter the password in password field
+4. Click on the Login button</t>
+  </si>
+  <si>
+    <t>Check if the system shows Invalid Login Credentials when you refresh the site and don’t enter a username and password.</t>
+  </si>
+  <si>
+    <t>1. User did not enter any of the required info and refresh the site</t>
+  </si>
+  <si>
+    <t>1. Open the browser
+2. Launch Rogationist College Student Portal 
+3. Refresh the Rogationist College Student Portal</t>
+  </si>
+  <si>
+    <t>Check if the systems Sign in button is working.</t>
+  </si>
+  <si>
+    <t>Click the Sign in button</t>
+  </si>
+  <si>
+    <t>1. Open the browser
+2. Launch Rogationist College Student Portal 
+3. Click the sign in button.</t>
+  </si>
+  <si>
+    <t>Sign in button is working</t>
+  </si>
+  <si>
+    <t>Sign in button is Working</t>
   </si>
 </sst>
 </file>
@@ -467,6 +542,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -484,12 +565,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -627,19 +702,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1091,16 +1166,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1552,7 +1627,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2019,7 +2094,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4941,10 +5016,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4993,7 +5068,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="C3" s="18"/>
       <c r="D3" s="18"/>
@@ -5007,7 +5082,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" s="18"/>
       <c r="D4" s="18"/>
@@ -5021,7 +5096,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="17"/>
       <c r="D5" s="17"/>
@@ -5035,7 +5110,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="17"/>
       <c r="D6" s="17"/>
@@ -5058,7 +5133,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>6</v>
@@ -5087,25 +5162,285 @@
         <v>1</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="E9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>21</v>
+      <c r="F9" s="5" t="s">
+        <v>22</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="H9" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>2</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="5" t="s">
-        <v>25</v>
+    </row>
+    <row r="11" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>3</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>5</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>6</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>7</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>8</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>10</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>11</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -5124,10 +5459,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E8E71CE-6838-4C65-BC4D-E6FB83E31F74}">
-  <dimension ref="A1:AM305"/>
+  <dimension ref="A1:AM291"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A27" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5141,19 +5476,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
-        <v>28</v>
+      <c r="A1" s="22" t="s">
+        <v>27</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -5226,20 +5561,20 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>79</v>
+      <c r="B3" s="23" t="s">
+        <v>64</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -5271,20 +5606,20 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>80</v>
+      <c r="B4" s="23" t="s">
+        <v>65</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
@@ -5316,24 +5651,24 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>83</v>
+      <c r="B5" s="24" t="s">
+        <v>68</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="16" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
-      <c r="H5" s="22" t="s">
-        <v>83</v>
+      <c r="H5" s="24" t="s">
+        <v>68</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -5365,22 +5700,22 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>84</v>
+      <c r="B6" s="24" t="s">
+        <v>69</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="16" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -5452,19 +5787,19 @@
       <c r="AM7" s="8"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>31</v>
+      <c r="A8" s="20" t="s">
+        <v>30</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -5537,14 +5872,14 @@
     </row>
     <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="B10" s="25">
-        <v>25</v>
+      <c r="B10" s="19">
+        <v>11</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -5582,14 +5917,14 @@
     </row>
     <row r="11" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
-      <c r="B11" s="25">
-        <v>3</v>
+      <c r="B11" s="19">
+        <v>0</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -5627,14 +5962,14 @@
     </row>
     <row r="12" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
-      <c r="B12" s="25">
-        <v>6</v>
+      <c r="B12" s="19">
+        <v>0</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -5672,14 +6007,14 @@
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="B13" s="25">
+      <c r="B13" s="19">
         <v>11</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -5717,14 +6052,14 @@
     </row>
     <row r="14" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
-      <c r="B14" s="25">
-        <v>3</v>
+      <c r="B14" s="19">
+        <v>0</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -5762,14 +6097,14 @@
     </row>
     <row r="15" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
-      <c r="B15" s="25">
-        <v>2</v>
+      <c r="B15" s="19">
+        <v>0</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -5847,24 +6182,24 @@
       <c r="AM16" s="8"/>
     </row>
     <row r="17" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="19" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
@@ -5875,14 +6210,14 @@
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
-      <c r="B21" s="25">
-        <v>10</v>
+      <c r="B21" s="19">
+        <v>0</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -5920,14 +6255,14 @@
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
-      <c r="B22" s="25">
-        <v>1</v>
+      <c r="B22" s="19">
+        <v>0</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -5965,14 +6300,14 @@
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
-      <c r="B23" s="25">
-        <v>2</v>
+      <c r="B23" s="19">
+        <v>0</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -6010,14 +6345,14 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
-      <c r="B24" s="25">
-        <v>3</v>
+      <c r="B24" s="19">
+        <v>0</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -6055,14 +6390,14 @@
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
-      <c r="B25" s="25">
-        <v>4</v>
+      <c r="B25" s="19">
+        <v>0</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -6345,19 +6680,19 @@
       <c r="AM31" s="8"/>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
-        <v>34</v>
+      <c r="A32" s="20" t="s">
+        <v>33</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
@@ -6391,24 +6726,24 @@
       <c r="A33" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>35</v>
+      <c r="B33" s="20" t="s">
+        <v>34</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="26" t="s">
-        <v>36</v>
+      <c r="H33" s="20" t="s">
+        <v>35</v>
       </c>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26" t="s">
+      <c r="I33" s="20"/>
+      <c r="J33" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="K33" s="26"/>
+      <c r="K33" s="20"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
@@ -6442,22 +6777,22 @@
       <c r="A34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>44</v>
+      <c r="B34" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
       <c r="G34" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H34" s="25" t="s">
-        <v>69</v>
+      <c r="H34" s="19" t="s">
+        <v>54</v>
       </c>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
@@ -6489,24 +6824,24 @@
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
+      <c r="B35" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H35" s="25" t="s">
-        <v>70</v>
+      <c r="H35" s="19" t="s">
+        <v>55</v>
       </c>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
@@ -6538,24 +6873,24 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
-      <c r="B36" s="25" t="s">
-        <v>44</v>
+      <c r="B36" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
       <c r="G36" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H36" s="25" t="s">
-        <v>71</v>
+      <c r="H36" s="19" t="s">
+        <v>56</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
@@ -6587,24 +6922,24 @@
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
-      <c r="B37" s="25" t="s">
-        <v>44</v>
+      <c r="B37" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
       <c r="G37" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H37" s="25" t="s">
-        <v>72</v>
+      <c r="H37" s="19" t="s">
+        <v>57</v>
       </c>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
@@ -6636,24 +6971,24 @@
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
-      <c r="B38" s="25" t="s">
-        <v>44</v>
+      <c r="B38" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
       <c r="G38" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H38" s="25" t="s">
-        <v>73</v>
+      <c r="H38" s="19" t="s">
+        <v>58</v>
       </c>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
@@ -6685,24 +7020,24 @@
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
-      <c r="B39" s="25" t="s">
-        <v>44</v>
+      <c r="B39" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H39" s="25" t="s">
-        <v>74</v>
+      <c r="H39" s="19" t="s">
+        <v>59</v>
       </c>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
@@ -6734,24 +7069,24 @@
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>44</v>
+      <c r="B40" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H40" s="25" t="s">
-        <v>75</v>
+      <c r="H40" s="19" t="s">
+        <v>60</v>
       </c>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -6783,24 +7118,24 @@
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
-      <c r="B41" s="25" t="s">
-        <v>44</v>
+      <c r="B41" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H41" s="25" t="s">
-        <v>76</v>
+      <c r="H41" s="19" t="s">
+        <v>61</v>
       </c>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
@@ -6832,24 +7167,24 @@
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
-      <c r="B42" s="25" t="s">
-        <v>44</v>
+      <c r="B42" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
       <c r="G42" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H42" s="25" t="s">
-        <v>77</v>
+      <c r="H42" s="19" t="s">
+        <v>62</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
@@ -6881,24 +7216,24 @@
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
-      <c r="B43" s="25" t="s">
-        <v>44</v>
+      <c r="B43" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
       <c r="G43" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H43" s="25" t="s">
-        <v>78</v>
+      <c r="H43" s="19" t="s">
+        <v>63</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
@@ -6930,22 +7265,22 @@
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
-      <c r="B44" s="25" t="s">
-        <v>44</v>
+      <c r="B44" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
       <c r="G44" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
@@ -6976,23 +7311,17 @@
       <c r="AM44" s="8"/>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
@@ -7023,23 +7352,17 @@
       <c r="AM45" s="8"/>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
@@ -7070,23 +7393,17 @@
       <c r="AM46" s="8"/>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
@@ -7117,23 +7434,17 @@
       <c r="AM47" s="8"/>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
       <c r="N48" s="8"/>
@@ -7164,23 +7475,17 @@
       <c r="AM48" s="8"/>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
       <c r="N49" s="8"/>
@@ -7211,23 +7516,17 @@
       <c r="AM49" s="8"/>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="25"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
@@ -7258,23 +7557,17 @@
       <c r="AM50" s="8"/>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="25"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
       <c r="N51" s="8"/>
@@ -7305,23 +7598,17 @@
       <c r="AM51" s="8"/>
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
       <c r="N52" s="8"/>
@@ -7352,23 +7639,17 @@
       <c r="AM52" s="8"/>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
       <c r="N53" s="8"/>
@@ -7399,23 +7680,17 @@
       <c r="AM53" s="8"/>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
       <c r="N54" s="8"/>
@@ -7446,23 +7721,17 @@
       <c r="AM54" s="8"/>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
       <c r="N55" s="8"/>
@@ -7493,23 +7762,17 @@
       <c r="AM55" s="8"/>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
-      <c r="J56" s="25"/>
-      <c r="K56" s="25"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
       <c r="N56" s="8"/>
@@ -7540,23 +7803,17 @@
       <c r="AM56" s="8"/>
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H57" s="25"/>
-      <c r="I57" s="25"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="25"/>
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
       <c r="N57" s="8"/>
@@ -7587,23 +7844,17 @@
       <c r="AM57" s="8"/>
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
-      <c r="J58" s="25"/>
-      <c r="K58" s="25"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
       <c r="N58" s="8"/>
@@ -17186,648 +17437,19 @@
       <c r="AL291" s="8"/>
       <c r="AM291" s="8"/>
     </row>
-    <row r="292" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A292" s="8"/>
-      <c r="B292" s="8"/>
-      <c r="C292" s="8"/>
-      <c r="D292" s="8"/>
-      <c r="E292" s="8"/>
-      <c r="F292" s="8"/>
-      <c r="G292" s="8"/>
-      <c r="H292" s="8"/>
-      <c r="I292" s="8"/>
-      <c r="J292" s="8"/>
-      <c r="K292" s="8"/>
-      <c r="L292" s="8"/>
-      <c r="M292" s="8"/>
-      <c r="N292" s="8"/>
-      <c r="O292" s="8"/>
-      <c r="P292" s="8"/>
-      <c r="Q292" s="8"/>
-      <c r="R292" s="8"/>
-      <c r="S292" s="8"/>
-      <c r="T292" s="8"/>
-      <c r="U292" s="8"/>
-      <c r="V292" s="8"/>
-      <c r="W292" s="8"/>
-      <c r="X292" s="8"/>
-      <c r="Y292" s="8"/>
-      <c r="Z292" s="8"/>
-      <c r="AA292" s="8"/>
-      <c r="AB292" s="8"/>
-      <c r="AC292" s="8"/>
-      <c r="AD292" s="8"/>
-      <c r="AE292" s="8"/>
-      <c r="AF292" s="8"/>
-      <c r="AG292" s="8"/>
-      <c r="AH292" s="8"/>
-      <c r="AI292" s="8"/>
-      <c r="AJ292" s="8"/>
-      <c r="AK292" s="8"/>
-      <c r="AL292" s="8"/>
-      <c r="AM292" s="8"/>
-    </row>
-    <row r="293" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A293" s="8"/>
-      <c r="B293" s="8"/>
-      <c r="C293" s="8"/>
-      <c r="D293" s="8"/>
-      <c r="E293" s="8"/>
-      <c r="F293" s="8"/>
-      <c r="G293" s="8"/>
-      <c r="H293" s="8"/>
-      <c r="I293" s="8"/>
-      <c r="J293" s="8"/>
-      <c r="K293" s="8"/>
-      <c r="L293" s="8"/>
-      <c r="M293" s="8"/>
-      <c r="N293" s="8"/>
-      <c r="O293" s="8"/>
-      <c r="P293" s="8"/>
-      <c r="Q293" s="8"/>
-      <c r="R293" s="8"/>
-      <c r="S293" s="8"/>
-      <c r="T293" s="8"/>
-      <c r="U293" s="8"/>
-      <c r="V293" s="8"/>
-      <c r="W293" s="8"/>
-      <c r="X293" s="8"/>
-      <c r="Y293" s="8"/>
-      <c r="Z293" s="8"/>
-      <c r="AA293" s="8"/>
-      <c r="AB293" s="8"/>
-      <c r="AC293" s="8"/>
-      <c r="AD293" s="8"/>
-      <c r="AE293" s="8"/>
-      <c r="AF293" s="8"/>
-      <c r="AG293" s="8"/>
-      <c r="AH293" s="8"/>
-      <c r="AI293" s="8"/>
-      <c r="AJ293" s="8"/>
-      <c r="AK293" s="8"/>
-      <c r="AL293" s="8"/>
-      <c r="AM293" s="8"/>
-    </row>
-    <row r="294" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A294" s="8"/>
-      <c r="B294" s="8"/>
-      <c r="C294" s="8"/>
-      <c r="D294" s="8"/>
-      <c r="E294" s="8"/>
-      <c r="F294" s="8"/>
-      <c r="G294" s="8"/>
-      <c r="H294" s="8"/>
-      <c r="I294" s="8"/>
-      <c r="J294" s="8"/>
-      <c r="K294" s="8"/>
-      <c r="L294" s="8"/>
-      <c r="M294" s="8"/>
-      <c r="N294" s="8"/>
-      <c r="O294" s="8"/>
-      <c r="P294" s="8"/>
-      <c r="Q294" s="8"/>
-      <c r="R294" s="8"/>
-      <c r="S294" s="8"/>
-      <c r="T294" s="8"/>
-      <c r="U294" s="8"/>
-      <c r="V294" s="8"/>
-      <c r="W294" s="8"/>
-      <c r="X294" s="8"/>
-      <c r="Y294" s="8"/>
-      <c r="Z294" s="8"/>
-      <c r="AA294" s="8"/>
-      <c r="AB294" s="8"/>
-      <c r="AC294" s="8"/>
-      <c r="AD294" s="8"/>
-      <c r="AE294" s="8"/>
-      <c r="AF294" s="8"/>
-      <c r="AG294" s="8"/>
-      <c r="AH294" s="8"/>
-      <c r="AI294" s="8"/>
-      <c r="AJ294" s="8"/>
-      <c r="AK294" s="8"/>
-      <c r="AL294" s="8"/>
-      <c r="AM294" s="8"/>
-    </row>
-    <row r="295" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A295" s="8"/>
-      <c r="B295" s="8"/>
-      <c r="C295" s="8"/>
-      <c r="D295" s="8"/>
-      <c r="E295" s="8"/>
-      <c r="F295" s="8"/>
-      <c r="G295" s="8"/>
-      <c r="H295" s="8"/>
-      <c r="I295" s="8"/>
-      <c r="J295" s="8"/>
-      <c r="K295" s="8"/>
-      <c r="L295" s="8"/>
-      <c r="M295" s="8"/>
-      <c r="N295" s="8"/>
-      <c r="O295" s="8"/>
-      <c r="P295" s="8"/>
-      <c r="Q295" s="8"/>
-      <c r="R295" s="8"/>
-      <c r="S295" s="8"/>
-      <c r="T295" s="8"/>
-      <c r="U295" s="8"/>
-      <c r="V295" s="8"/>
-      <c r="W295" s="8"/>
-      <c r="X295" s="8"/>
-      <c r="Y295" s="8"/>
-      <c r="Z295" s="8"/>
-      <c r="AA295" s="8"/>
-      <c r="AB295" s="8"/>
-      <c r="AC295" s="8"/>
-      <c r="AD295" s="8"/>
-      <c r="AE295" s="8"/>
-      <c r="AF295" s="8"/>
-      <c r="AG295" s="8"/>
-      <c r="AH295" s="8"/>
-      <c r="AI295" s="8"/>
-      <c r="AJ295" s="8"/>
-      <c r="AK295" s="8"/>
-      <c r="AL295" s="8"/>
-      <c r="AM295" s="8"/>
-    </row>
-    <row r="296" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A296" s="8"/>
-      <c r="B296" s="8"/>
-      <c r="C296" s="8"/>
-      <c r="D296" s="8"/>
-      <c r="E296" s="8"/>
-      <c r="F296" s="8"/>
-      <c r="G296" s="8"/>
-      <c r="H296" s="8"/>
-      <c r="I296" s="8"/>
-      <c r="J296" s="8"/>
-      <c r="K296" s="8"/>
-      <c r="L296" s="8"/>
-      <c r="M296" s="8"/>
-      <c r="N296" s="8"/>
-      <c r="O296" s="8"/>
-      <c r="P296" s="8"/>
-      <c r="Q296" s="8"/>
-      <c r="R296" s="8"/>
-      <c r="S296" s="8"/>
-      <c r="T296" s="8"/>
-      <c r="U296" s="8"/>
-      <c r="V296" s="8"/>
-      <c r="W296" s="8"/>
-      <c r="X296" s="8"/>
-      <c r="Y296" s="8"/>
-      <c r="Z296" s="8"/>
-      <c r="AA296" s="8"/>
-      <c r="AB296" s="8"/>
-      <c r="AC296" s="8"/>
-      <c r="AD296" s="8"/>
-      <c r="AE296" s="8"/>
-      <c r="AF296" s="8"/>
-      <c r="AG296" s="8"/>
-      <c r="AH296" s="8"/>
-      <c r="AI296" s="8"/>
-      <c r="AJ296" s="8"/>
-      <c r="AK296" s="8"/>
-      <c r="AL296" s="8"/>
-      <c r="AM296" s="8"/>
-    </row>
-    <row r="297" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A297" s="8"/>
-      <c r="B297" s="8"/>
-      <c r="C297" s="8"/>
-      <c r="D297" s="8"/>
-      <c r="E297" s="8"/>
-      <c r="F297" s="8"/>
-      <c r="G297" s="8"/>
-      <c r="H297" s="8"/>
-      <c r="I297" s="8"/>
-      <c r="J297" s="8"/>
-      <c r="K297" s="8"/>
-      <c r="L297" s="8"/>
-      <c r="M297" s="8"/>
-      <c r="N297" s="8"/>
-      <c r="O297" s="8"/>
-      <c r="P297" s="8"/>
-      <c r="Q297" s="8"/>
-      <c r="R297" s="8"/>
-      <c r="S297" s="8"/>
-      <c r="T297" s="8"/>
-      <c r="U297" s="8"/>
-      <c r="V297" s="8"/>
-      <c r="W297" s="8"/>
-      <c r="X297" s="8"/>
-      <c r="Y297" s="8"/>
-      <c r="Z297" s="8"/>
-      <c r="AA297" s="8"/>
-      <c r="AB297" s="8"/>
-      <c r="AC297" s="8"/>
-      <c r="AD297" s="8"/>
-      <c r="AE297" s="8"/>
-      <c r="AF297" s="8"/>
-      <c r="AG297" s="8"/>
-      <c r="AH297" s="8"/>
-      <c r="AI297" s="8"/>
-      <c r="AJ297" s="8"/>
-      <c r="AK297" s="8"/>
-      <c r="AL297" s="8"/>
-      <c r="AM297" s="8"/>
-    </row>
-    <row r="298" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A298" s="8"/>
-      <c r="B298" s="8"/>
-      <c r="C298" s="8"/>
-      <c r="D298" s="8"/>
-      <c r="E298" s="8"/>
-      <c r="F298" s="8"/>
-      <c r="G298" s="8"/>
-      <c r="H298" s="8"/>
-      <c r="I298" s="8"/>
-      <c r="J298" s="8"/>
-      <c r="K298" s="8"/>
-      <c r="L298" s="8"/>
-      <c r="M298" s="8"/>
-      <c r="N298" s="8"/>
-      <c r="O298" s="8"/>
-      <c r="P298" s="8"/>
-      <c r="Q298" s="8"/>
-      <c r="R298" s="8"/>
-      <c r="S298" s="8"/>
-      <c r="T298" s="8"/>
-      <c r="U298" s="8"/>
-      <c r="V298" s="8"/>
-      <c r="W298" s="8"/>
-      <c r="X298" s="8"/>
-      <c r="Y298" s="8"/>
-      <c r="Z298" s="8"/>
-      <c r="AA298" s="8"/>
-      <c r="AB298" s="8"/>
-      <c r="AC298" s="8"/>
-      <c r="AD298" s="8"/>
-      <c r="AE298" s="8"/>
-      <c r="AF298" s="8"/>
-      <c r="AG298" s="8"/>
-      <c r="AH298" s="8"/>
-      <c r="AI298" s="8"/>
-      <c r="AJ298" s="8"/>
-      <c r="AK298" s="8"/>
-      <c r="AL298" s="8"/>
-      <c r="AM298" s="8"/>
-    </row>
-    <row r="299" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A299" s="8"/>
-      <c r="B299" s="8"/>
-      <c r="C299" s="8"/>
-      <c r="D299" s="8"/>
-      <c r="E299" s="8"/>
-      <c r="F299" s="8"/>
-      <c r="G299" s="8"/>
-      <c r="H299" s="8"/>
-      <c r="I299" s="8"/>
-      <c r="J299" s="8"/>
-      <c r="K299" s="8"/>
-      <c r="L299" s="8"/>
-      <c r="M299" s="8"/>
-      <c r="N299" s="8"/>
-      <c r="O299" s="8"/>
-      <c r="P299" s="8"/>
-      <c r="Q299" s="8"/>
-      <c r="R299" s="8"/>
-      <c r="S299" s="8"/>
-      <c r="T299" s="8"/>
-      <c r="U299" s="8"/>
-      <c r="V299" s="8"/>
-      <c r="W299" s="8"/>
-      <c r="X299" s="8"/>
-      <c r="Y299" s="8"/>
-      <c r="Z299" s="8"/>
-      <c r="AA299" s="8"/>
-      <c r="AB299" s="8"/>
-      <c r="AC299" s="8"/>
-      <c r="AD299" s="8"/>
-      <c r="AE299" s="8"/>
-      <c r="AF299" s="8"/>
-      <c r="AG299" s="8"/>
-      <c r="AH299" s="8"/>
-      <c r="AI299" s="8"/>
-      <c r="AJ299" s="8"/>
-      <c r="AK299" s="8"/>
-      <c r="AL299" s="8"/>
-      <c r="AM299" s="8"/>
-    </row>
-    <row r="300" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A300" s="8"/>
-      <c r="B300" s="8"/>
-      <c r="C300" s="8"/>
-      <c r="D300" s="8"/>
-      <c r="E300" s="8"/>
-      <c r="F300" s="8"/>
-      <c r="G300" s="8"/>
-      <c r="H300" s="8"/>
-      <c r="I300" s="8"/>
-      <c r="J300" s="8"/>
-      <c r="K300" s="8"/>
-      <c r="L300" s="8"/>
-      <c r="M300" s="8"/>
-      <c r="N300" s="8"/>
-      <c r="O300" s="8"/>
-      <c r="P300" s="8"/>
-      <c r="Q300" s="8"/>
-      <c r="R300" s="8"/>
-      <c r="S300" s="8"/>
-      <c r="T300" s="8"/>
-      <c r="U300" s="8"/>
-      <c r="V300" s="8"/>
-      <c r="W300" s="8"/>
-      <c r="X300" s="8"/>
-      <c r="Y300" s="8"/>
-      <c r="Z300" s="8"/>
-      <c r="AA300" s="8"/>
-      <c r="AB300" s="8"/>
-      <c r="AC300" s="8"/>
-      <c r="AD300" s="8"/>
-      <c r="AE300" s="8"/>
-      <c r="AF300" s="8"/>
-      <c r="AG300" s="8"/>
-      <c r="AH300" s="8"/>
-      <c r="AI300" s="8"/>
-      <c r="AJ300" s="8"/>
-      <c r="AK300" s="8"/>
-      <c r="AL300" s="8"/>
-      <c r="AM300" s="8"/>
-    </row>
-    <row r="301" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A301" s="8"/>
-      <c r="B301" s="8"/>
-      <c r="C301" s="8"/>
-      <c r="D301" s="8"/>
-      <c r="E301" s="8"/>
-      <c r="F301" s="8"/>
-      <c r="G301" s="8"/>
-      <c r="H301" s="8"/>
-      <c r="I301" s="8"/>
-      <c r="J301" s="8"/>
-      <c r="K301" s="8"/>
-      <c r="L301" s="8"/>
-      <c r="M301" s="8"/>
-      <c r="N301" s="8"/>
-      <c r="O301" s="8"/>
-      <c r="P301" s="8"/>
-      <c r="Q301" s="8"/>
-      <c r="R301" s="8"/>
-      <c r="S301" s="8"/>
-      <c r="T301" s="8"/>
-      <c r="U301" s="8"/>
-      <c r="V301" s="8"/>
-      <c r="W301" s="8"/>
-      <c r="X301" s="8"/>
-      <c r="Y301" s="8"/>
-      <c r="Z301" s="8"/>
-      <c r="AA301" s="8"/>
-      <c r="AB301" s="8"/>
-      <c r="AC301" s="8"/>
-      <c r="AD301" s="8"/>
-      <c r="AE301" s="8"/>
-      <c r="AF301" s="8"/>
-      <c r="AG301" s="8"/>
-      <c r="AH301" s="8"/>
-      <c r="AI301" s="8"/>
-      <c r="AJ301" s="8"/>
-      <c r="AK301" s="8"/>
-      <c r="AL301" s="8"/>
-      <c r="AM301" s="8"/>
-    </row>
-    <row r="302" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A302" s="8"/>
-      <c r="B302" s="8"/>
-      <c r="C302" s="8"/>
-      <c r="D302" s="8"/>
-      <c r="E302" s="8"/>
-      <c r="F302" s="8"/>
-      <c r="G302" s="8"/>
-      <c r="H302" s="8"/>
-      <c r="I302" s="8"/>
-      <c r="J302" s="8"/>
-      <c r="K302" s="8"/>
-      <c r="L302" s="8"/>
-      <c r="M302" s="8"/>
-      <c r="N302" s="8"/>
-      <c r="O302" s="8"/>
-      <c r="P302" s="8"/>
-      <c r="Q302" s="8"/>
-      <c r="R302" s="8"/>
-      <c r="S302" s="8"/>
-      <c r="T302" s="8"/>
-      <c r="U302" s="8"/>
-      <c r="V302" s="8"/>
-      <c r="W302" s="8"/>
-      <c r="X302" s="8"/>
-      <c r="Y302" s="8"/>
-      <c r="Z302" s="8"/>
-      <c r="AA302" s="8"/>
-      <c r="AB302" s="8"/>
-      <c r="AC302" s="8"/>
-      <c r="AD302" s="8"/>
-      <c r="AE302" s="8"/>
-      <c r="AF302" s="8"/>
-      <c r="AG302" s="8"/>
-      <c r="AH302" s="8"/>
-      <c r="AI302" s="8"/>
-      <c r="AJ302" s="8"/>
-      <c r="AK302" s="8"/>
-      <c r="AL302" s="8"/>
-      <c r="AM302" s="8"/>
-    </row>
-    <row r="303" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A303" s="8"/>
-      <c r="B303" s="8"/>
-      <c r="C303" s="8"/>
-      <c r="D303" s="8"/>
-      <c r="E303" s="8"/>
-      <c r="F303" s="8"/>
-      <c r="G303" s="8"/>
-      <c r="H303" s="8"/>
-      <c r="I303" s="8"/>
-      <c r="J303" s="8"/>
-      <c r="K303" s="8"/>
-      <c r="L303" s="8"/>
-      <c r="M303" s="8"/>
-      <c r="N303" s="8"/>
-      <c r="O303" s="8"/>
-      <c r="P303" s="8"/>
-      <c r="Q303" s="8"/>
-      <c r="R303" s="8"/>
-      <c r="S303" s="8"/>
-      <c r="T303" s="8"/>
-      <c r="U303" s="8"/>
-      <c r="V303" s="8"/>
-      <c r="W303" s="8"/>
-      <c r="X303" s="8"/>
-      <c r="Y303" s="8"/>
-      <c r="Z303" s="8"/>
-      <c r="AA303" s="8"/>
-      <c r="AB303" s="8"/>
-      <c r="AC303" s="8"/>
-      <c r="AD303" s="8"/>
-      <c r="AE303" s="8"/>
-      <c r="AF303" s="8"/>
-      <c r="AG303" s="8"/>
-      <c r="AH303" s="8"/>
-      <c r="AI303" s="8"/>
-      <c r="AJ303" s="8"/>
-      <c r="AK303" s="8"/>
-      <c r="AL303" s="8"/>
-      <c r="AM303" s="8"/>
-    </row>
-    <row r="304" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A304" s="8"/>
-      <c r="B304" s="8"/>
-      <c r="C304" s="8"/>
-      <c r="D304" s="8"/>
-      <c r="E304" s="8"/>
-      <c r="F304" s="8"/>
-      <c r="G304" s="8"/>
-      <c r="H304" s="8"/>
-      <c r="I304" s="8"/>
-      <c r="J304" s="8"/>
-      <c r="K304" s="8"/>
-      <c r="L304" s="8"/>
-      <c r="M304" s="8"/>
-      <c r="N304" s="8"/>
-      <c r="O304" s="8"/>
-      <c r="P304" s="8"/>
-      <c r="Q304" s="8"/>
-      <c r="R304" s="8"/>
-      <c r="S304" s="8"/>
-      <c r="T304" s="8"/>
-      <c r="U304" s="8"/>
-      <c r="V304" s="8"/>
-      <c r="W304" s="8"/>
-      <c r="X304" s="8"/>
-      <c r="Y304" s="8"/>
-      <c r="Z304" s="8"/>
-      <c r="AA304" s="8"/>
-      <c r="AB304" s="8"/>
-      <c r="AC304" s="8"/>
-      <c r="AD304" s="8"/>
-      <c r="AE304" s="8"/>
-      <c r="AF304" s="8"/>
-      <c r="AG304" s="8"/>
-      <c r="AH304" s="8"/>
-      <c r="AI304" s="8"/>
-      <c r="AJ304" s="8"/>
-      <c r="AK304" s="8"/>
-      <c r="AL304" s="8"/>
-      <c r="AM304" s="8"/>
-    </row>
-    <row r="305" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A305" s="8"/>
-      <c r="B305" s="8"/>
-      <c r="C305" s="8"/>
-      <c r="D305" s="8"/>
-      <c r="E305" s="8"/>
-      <c r="F305" s="8"/>
-      <c r="G305" s="8"/>
-      <c r="H305" s="8"/>
-      <c r="I305" s="8"/>
-      <c r="J305" s="8"/>
-      <c r="K305" s="8"/>
-      <c r="L305" s="8"/>
-      <c r="M305" s="8"/>
-      <c r="N305" s="8"/>
-      <c r="O305" s="8"/>
-      <c r="P305" s="8"/>
-      <c r="Q305" s="8"/>
-      <c r="R305" s="8"/>
-      <c r="S305" s="8"/>
-      <c r="T305" s="8"/>
-      <c r="U305" s="8"/>
-      <c r="V305" s="8"/>
-      <c r="W305" s="8"/>
-      <c r="X305" s="8"/>
-      <c r="Y305" s="8"/>
-      <c r="Z305" s="8"/>
-      <c r="AA305" s="8"/>
-      <c r="AB305" s="8"/>
-      <c r="AC305" s="8"/>
-      <c r="AD305" s="8"/>
-      <c r="AE305" s="8"/>
-      <c r="AF305" s="8"/>
-      <c r="AG305" s="8"/>
-      <c r="AH305" s="8"/>
-      <c r="AI305" s="8"/>
-      <c r="AJ305" s="8"/>
-      <c r="AK305" s="8"/>
-      <c r="AL305" s="8"/>
-      <c r="AM305" s="8"/>
-    </row>
   </sheetData>
-  <mergeCells count="101">
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="J57:K57"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B37:F37"/>
+  <mergeCells count="59">
+    <mergeCell ref="B17:E17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="J36:K36"/>
     <mergeCell ref="A8:K8"/>
@@ -17852,17 +17474,30 @@
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="J35:K35"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="B44:F44"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17872,10 +17507,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C43A335C-A6C0-41AD-B9C4-8C4636D87553}">
-  <dimension ref="A1:AM305"/>
+  <dimension ref="A1:AM291"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView topLeftCell="A33" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17889,19 +17524,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
-        <v>28</v>
+      <c r="A1" s="22" t="s">
+        <v>27</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
@@ -17974,20 +17609,20 @@
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
-      <c r="B3" s="21" t="s">
-        <v>79</v>
+      <c r="B3" s="23" t="s">
+        <v>64</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -18019,20 +17654,20 @@
     </row>
     <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
-      <c r="B4" s="21" t="s">
-        <v>80</v>
+      <c r="B4" s="23" t="s">
+        <v>65</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
@@ -18064,24 +17699,24 @@
     </row>
     <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
-      <c r="B5" s="22" t="s">
-        <v>83</v>
+      <c r="B5" s="24" t="s">
+        <v>68</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="24"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="26"/>
       <c r="G5" s="16" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
-      <c r="H5" s="22" t="s">
-        <v>83</v>
+      <c r="H5" s="24" t="s">
+        <v>68</v>
       </c>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26"/>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -18113,22 +17748,22 @@
     </row>
     <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>84</v>
+      <c r="B6" s="24" t="s">
+        <v>69</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="24"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="16" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="26"/>
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
@@ -18200,19 +17835,19 @@
       <c r="AM7" s="8"/>
     </row>
     <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
-        <v>31</v>
+      <c r="A8" s="20" t="s">
+        <v>30</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
@@ -18285,14 +17920,14 @@
     </row>
     <row r="10" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
-      <c r="B10" s="25">
-        <v>25</v>
+      <c r="B10" s="19">
+        <v>11</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -18330,14 +17965,14 @@
     </row>
     <row r="11" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
-      <c r="B11" s="25">
+      <c r="B11" s="19">
         <v>0</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -18375,14 +18010,14 @@
     </row>
     <row r="12" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
-      <c r="B12" s="25">
+      <c r="B12" s="19">
         <v>0</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -18420,14 +18055,14 @@
     </row>
     <row r="13" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="B13" s="25">
-        <v>25</v>
+      <c r="B13" s="19">
+        <v>11</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -18465,14 +18100,14 @@
     </row>
     <row r="14" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
-      <c r="B14" s="25">
+      <c r="B14" s="19">
         <v>0</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -18510,14 +18145,14 @@
     </row>
     <row r="15" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
-      <c r="B15" s="25">
+      <c r="B15" s="19">
         <v>0</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -18595,24 +18230,24 @@
       <c r="AM16" s="8"/>
     </row>
     <row r="17" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
     </row>
     <row r="18" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="19"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
     </row>
     <row r="19" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
@@ -18623,14 +18258,14 @@
     </row>
     <row r="21" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
-      <c r="B21" s="25">
-        <v>10</v>
+      <c r="B21" s="19">
+        <v>0</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -18668,14 +18303,14 @@
     </row>
     <row r="22" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A22" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
-      <c r="B22" s="25">
+      <c r="B22" s="19">
         <v>0</v>
       </c>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -18713,14 +18348,14 @@
     </row>
     <row r="23" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A23" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
-      <c r="B23" s="25">
+      <c r="B23" s="19">
         <v>0</v>
       </c>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -18758,14 +18393,14 @@
     </row>
     <row r="24" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A24" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
-      <c r="B24" s="25">
+      <c r="B24" s="19">
         <v>0</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -18803,14 +18438,14 @@
     </row>
     <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
-      <c r="B25" s="25">
-        <v>10</v>
+      <c r="B25" s="19">
+        <v>0</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -19093,19 +18728,19 @@
       <c r="AM31" s="8"/>
     </row>
     <row r="32" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
-        <v>34</v>
+      <c r="A32" s="20" t="s">
+        <v>33</v>
       </c>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="20"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
@@ -19139,24 +18774,24 @@
       <c r="A33" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>35</v>
+      <c r="B33" s="20" t="s">
+        <v>34</v>
       </c>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
       <c r="G33" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H33" s="26" t="s">
-        <v>36</v>
+      <c r="H33" s="20" t="s">
+        <v>35</v>
       </c>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26" t="s">
+      <c r="I33" s="20"/>
+      <c r="J33" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="K33" s="26"/>
+      <c r="K33" s="20"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
@@ -19190,22 +18825,22 @@
       <c r="A34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B34" s="25" t="s">
-        <v>44</v>
+      <c r="B34" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C34" s="25"/>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="25"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
       <c r="G34" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H34" s="25" t="s">
-        <v>69</v>
+      <c r="H34" s="19" t="s">
+        <v>54</v>
       </c>
-      <c r="I34" s="25"/>
-      <c r="J34" s="25"/>
-      <c r="K34" s="25"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
@@ -19237,24 +18872,24 @@
     </row>
     <row r="35" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B35" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="25"/>
-      <c r="D35" s="25"/>
-      <c r="E35" s="25"/>
-      <c r="F35" s="25"/>
+      <c r="B35" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H35" s="25" t="s">
-        <v>70</v>
+      <c r="H35" s="19" t="s">
+        <v>55</v>
       </c>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
       <c r="L35" s="8"/>
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
@@ -19286,24 +18921,24 @@
     </row>
     <row r="36" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
-      <c r="B36" s="25" t="s">
-        <v>44</v>
+      <c r="B36" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C36" s="25"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="25"/>
-      <c r="F36" s="25"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
       <c r="G36" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H36" s="25" t="s">
-        <v>71</v>
+      <c r="H36" s="19" t="s">
+        <v>56</v>
       </c>
-      <c r="I36" s="25"/>
-      <c r="J36" s="25"/>
-      <c r="K36" s="25"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
       <c r="L36" s="8"/>
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
@@ -19335,24 +18970,24 @@
     </row>
     <row r="37" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
-      <c r="B37" s="25" t="s">
-        <v>44</v>
+      <c r="B37" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C37" s="25"/>
-      <c r="D37" s="25"/>
-      <c r="E37" s="25"/>
-      <c r="F37" s="25"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="19"/>
       <c r="G37" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H37" s="25" t="s">
-        <v>72</v>
+      <c r="H37" s="19" t="s">
+        <v>57</v>
       </c>
-      <c r="I37" s="25"/>
-      <c r="J37" s="25"/>
-      <c r="K37" s="25"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
       <c r="L37" s="8"/>
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
@@ -19384,24 +19019,24 @@
     </row>
     <row r="38" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
-      <c r="B38" s="25" t="s">
-        <v>44</v>
+      <c r="B38" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
+      <c r="C38" s="19"/>
+      <c r="D38" s="19"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="19"/>
       <c r="G38" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H38" s="25" t="s">
-        <v>73</v>
+      <c r="H38" s="19" t="s">
+        <v>58</v>
       </c>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
@@ -19433,24 +19068,24 @@
     </row>
     <row r="39" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
-      <c r="B39" s="25" t="s">
-        <v>44</v>
+      <c r="B39" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
+      <c r="C39" s="19"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="19"/>
       <c r="G39" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H39" s="25" t="s">
-        <v>74</v>
+      <c r="H39" s="19" t="s">
+        <v>59</v>
       </c>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
       <c r="L39" s="8"/>
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
@@ -19482,24 +19117,24 @@
     </row>
     <row r="40" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
-      <c r="B40" s="25" t="s">
-        <v>44</v>
+      <c r="B40" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
+      <c r="C40" s="19"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="19"/>
       <c r="G40" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H40" s="25" t="s">
-        <v>75</v>
+      <c r="H40" s="19" t="s">
+        <v>60</v>
       </c>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
@@ -19531,24 +19166,24 @@
     </row>
     <row r="41" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
-      <c r="B41" s="25" t="s">
-        <v>44</v>
+      <c r="B41" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="19"/>
       <c r="G41" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H41" s="25" t="s">
-        <v>76</v>
+      <c r="H41" s="19" t="s">
+        <v>61</v>
       </c>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
+      <c r="I41" s="19"/>
+      <c r="J41" s="19"/>
+      <c r="K41" s="19"/>
       <c r="L41" s="8"/>
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
@@ -19580,24 +19215,24 @@
     </row>
     <row r="42" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
-      <c r="B42" s="25" t="s">
-        <v>44</v>
+      <c r="B42" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="19"/>
+      <c r="F42" s="19"/>
       <c r="G42" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H42" s="25" t="s">
-        <v>77</v>
+      <c r="H42" s="19" t="s">
+        <v>62</v>
       </c>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
+      <c r="I42" s="19"/>
+      <c r="J42" s="19"/>
+      <c r="K42" s="19"/>
       <c r="L42" s="8"/>
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
@@ -19629,24 +19264,24 @@
     </row>
     <row r="43" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
-      <c r="B43" s="25" t="s">
-        <v>44</v>
+      <c r="B43" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
       <c r="G43" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H43" s="25" t="s">
-        <v>78</v>
+      <c r="H43" s="19" t="s">
+        <v>63</v>
       </c>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="19"/>
+      <c r="K43" s="19"/>
       <c r="L43" s="8"/>
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
@@ -19678,22 +19313,22 @@
     </row>
     <row r="44" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
-      <c r="B44" s="25" t="s">
-        <v>44</v>
+      <c r="B44" s="19" t="s">
+        <v>43</v>
       </c>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
       <c r="G44" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+      <c r="K44" s="19"/>
       <c r="L44" s="8"/>
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
@@ -19724,23 +19359,17 @@
       <c r="AM44" s="8"/>
     </row>
     <row r="45" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A45" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B45" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+      <c r="E45" s="8"/>
+      <c r="F45" s="8"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
       <c r="L45" s="8"/>
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
@@ -19771,23 +19400,17 @@
       <c r="AM45" s="8"/>
     </row>
     <row r="46" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="8"/>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
       <c r="L46" s="8"/>
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
@@ -19818,23 +19441,17 @@
       <c r="AM46" s="8"/>
     </row>
     <row r="47" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B47" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="8"/>
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
       <c r="L47" s="8"/>
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
@@ -19865,23 +19482,17 @@
       <c r="AM47" s="8"/>
     </row>
     <row r="48" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B48" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="8"/>
+      <c r="F48" s="8"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
       <c r="L48" s="8"/>
       <c r="M48" s="8"/>
       <c r="N48" s="8"/>
@@ -19912,23 +19523,17 @@
       <c r="AM48" s="8"/>
     </row>
     <row r="49" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A49" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B49" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
       <c r="L49" s="8"/>
       <c r="M49" s="8"/>
       <c r="N49" s="8"/>
@@ -19959,23 +19564,17 @@
       <c r="AM49" s="8"/>
     </row>
     <row r="50" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="25"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="8"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
       <c r="L50" s="8"/>
       <c r="M50" s="8"/>
       <c r="N50" s="8"/>
@@ -20006,23 +19605,17 @@
       <c r="AM50" s="8"/>
     </row>
     <row r="51" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A51" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="25"/>
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
       <c r="L51" s="8"/>
       <c r="M51" s="8"/>
       <c r="N51" s="8"/>
@@ -20053,23 +19646,17 @@
       <c r="AM51" s="8"/>
     </row>
     <row r="52" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="8"/>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
       <c r="L52" s="8"/>
       <c r="M52" s="8"/>
       <c r="N52" s="8"/>
@@ -20100,23 +19687,17 @@
       <c r="AM52" s="8"/>
     </row>
     <row r="53" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A53" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="B53" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="8"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
       <c r="L53" s="8"/>
       <c r="M53" s="8"/>
       <c r="N53" s="8"/>
@@ -20147,23 +19728,17 @@
       <c r="AM53" s="8"/>
     </row>
     <row r="54" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
       <c r="L54" s="8"/>
       <c r="M54" s="8"/>
       <c r="N54" s="8"/>
@@ -20194,23 +19769,17 @@
       <c r="AM54" s="8"/>
     </row>
     <row r="55" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="B55" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="25"/>
-      <c r="D55" s="25"/>
-      <c r="E55" s="25"/>
-      <c r="F55" s="25"/>
-      <c r="G55" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H55" s="25"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="25"/>
-      <c r="K55" s="25"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
       <c r="L55" s="8"/>
       <c r="M55" s="8"/>
       <c r="N55" s="8"/>
@@ -20241,23 +19810,17 @@
       <c r="AM55" s="8"/>
     </row>
     <row r="56" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B56" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C56" s="25"/>
-      <c r="D56" s="25"/>
-      <c r="E56" s="25"/>
-      <c r="F56" s="25"/>
-      <c r="G56" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H56" s="25"/>
-      <c r="I56" s="25"/>
-      <c r="J56" s="25"/>
-      <c r="K56" s="25"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="8"/>
+      <c r="E56" s="8"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
       <c r="L56" s="8"/>
       <c r="M56" s="8"/>
       <c r="N56" s="8"/>
@@ -20288,23 +19851,17 @@
       <c r="AM56" s="8"/>
     </row>
     <row r="57" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B57" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C57" s="25"/>
-      <c r="D57" s="25"/>
-      <c r="E57" s="25"/>
-      <c r="F57" s="25"/>
-      <c r="G57" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H57" s="25"/>
-      <c r="I57" s="25"/>
-      <c r="J57" s="25"/>
-      <c r="K57" s="25"/>
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
+      <c r="D57" s="8"/>
+      <c r="E57" s="8"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
       <c r="L57" s="8"/>
       <c r="M57" s="8"/>
       <c r="N57" s="8"/>
@@ -20335,23 +19892,17 @@
       <c r="AM57" s="8"/>
     </row>
     <row r="58" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="B58" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="C58" s="25"/>
-      <c r="D58" s="25"/>
-      <c r="E58" s="25"/>
-      <c r="F58" s="25"/>
-      <c r="G58" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H58" s="25"/>
-      <c r="I58" s="25"/>
-      <c r="J58" s="25"/>
-      <c r="K58" s="25"/>
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="8"/>
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
       <c r="N58" s="8"/>
@@ -29934,601 +29485,35 @@
       <c r="AL291" s="8"/>
       <c r="AM291" s="8"/>
     </row>
-    <row r="292" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A292" s="8"/>
-      <c r="B292" s="8"/>
-      <c r="C292" s="8"/>
-      <c r="D292" s="8"/>
-      <c r="E292" s="8"/>
-      <c r="F292" s="8"/>
-      <c r="G292" s="8"/>
-      <c r="H292" s="8"/>
-      <c r="I292" s="8"/>
-      <c r="J292" s="8"/>
-      <c r="K292" s="8"/>
-      <c r="L292" s="8"/>
-      <c r="M292" s="8"/>
-      <c r="N292" s="8"/>
-      <c r="O292" s="8"/>
-      <c r="P292" s="8"/>
-      <c r="Q292" s="8"/>
-      <c r="R292" s="8"/>
-      <c r="S292" s="8"/>
-      <c r="T292" s="8"/>
-      <c r="U292" s="8"/>
-      <c r="V292" s="8"/>
-      <c r="W292" s="8"/>
-      <c r="X292" s="8"/>
-      <c r="Y292" s="8"/>
-      <c r="Z292" s="8"/>
-      <c r="AA292" s="8"/>
-      <c r="AB292" s="8"/>
-      <c r="AC292" s="8"/>
-      <c r="AD292" s="8"/>
-      <c r="AE292" s="8"/>
-      <c r="AF292" s="8"/>
-      <c r="AG292" s="8"/>
-      <c r="AH292" s="8"/>
-      <c r="AI292" s="8"/>
-      <c r="AJ292" s="8"/>
-      <c r="AK292" s="8"/>
-      <c r="AL292" s="8"/>
-      <c r="AM292" s="8"/>
-    </row>
-    <row r="293" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A293" s="8"/>
-      <c r="B293" s="8"/>
-      <c r="C293" s="8"/>
-      <c r="D293" s="8"/>
-      <c r="E293" s="8"/>
-      <c r="F293" s="8"/>
-      <c r="G293" s="8"/>
-      <c r="H293" s="8"/>
-      <c r="I293" s="8"/>
-      <c r="J293" s="8"/>
-      <c r="K293" s="8"/>
-      <c r="L293" s="8"/>
-      <c r="M293" s="8"/>
-      <c r="N293" s="8"/>
-      <c r="O293" s="8"/>
-      <c r="P293" s="8"/>
-      <c r="Q293" s="8"/>
-      <c r="R293" s="8"/>
-      <c r="S293" s="8"/>
-      <c r="T293" s="8"/>
-      <c r="U293" s="8"/>
-      <c r="V293" s="8"/>
-      <c r="W293" s="8"/>
-      <c r="X293" s="8"/>
-      <c r="Y293" s="8"/>
-      <c r="Z293" s="8"/>
-      <c r="AA293" s="8"/>
-      <c r="AB293" s="8"/>
-      <c r="AC293" s="8"/>
-      <c r="AD293" s="8"/>
-      <c r="AE293" s="8"/>
-      <c r="AF293" s="8"/>
-      <c r="AG293" s="8"/>
-      <c r="AH293" s="8"/>
-      <c r="AI293" s="8"/>
-      <c r="AJ293" s="8"/>
-      <c r="AK293" s="8"/>
-      <c r="AL293" s="8"/>
-      <c r="AM293" s="8"/>
-    </row>
-    <row r="294" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A294" s="8"/>
-      <c r="B294" s="8"/>
-      <c r="C294" s="8"/>
-      <c r="D294" s="8"/>
-      <c r="E294" s="8"/>
-      <c r="F294" s="8"/>
-      <c r="G294" s="8"/>
-      <c r="H294" s="8"/>
-      <c r="I294" s="8"/>
-      <c r="J294" s="8"/>
-      <c r="K294" s="8"/>
-      <c r="L294" s="8"/>
-      <c r="M294" s="8"/>
-      <c r="N294" s="8"/>
-      <c r="O294" s="8"/>
-      <c r="P294" s="8"/>
-      <c r="Q294" s="8"/>
-      <c r="R294" s="8"/>
-      <c r="S294" s="8"/>
-      <c r="T294" s="8"/>
-      <c r="U294" s="8"/>
-      <c r="V294" s="8"/>
-      <c r="W294" s="8"/>
-      <c r="X294" s="8"/>
-      <c r="Y294" s="8"/>
-      <c r="Z294" s="8"/>
-      <c r="AA294" s="8"/>
-      <c r="AB294" s="8"/>
-      <c r="AC294" s="8"/>
-      <c r="AD294" s="8"/>
-      <c r="AE294" s="8"/>
-      <c r="AF294" s="8"/>
-      <c r="AG294" s="8"/>
-      <c r="AH294" s="8"/>
-      <c r="AI294" s="8"/>
-      <c r="AJ294" s="8"/>
-      <c r="AK294" s="8"/>
-      <c r="AL294" s="8"/>
-      <c r="AM294" s="8"/>
-    </row>
-    <row r="295" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A295" s="8"/>
-      <c r="B295" s="8"/>
-      <c r="C295" s="8"/>
-      <c r="D295" s="8"/>
-      <c r="E295" s="8"/>
-      <c r="F295" s="8"/>
-      <c r="G295" s="8"/>
-      <c r="H295" s="8"/>
-      <c r="I295" s="8"/>
-      <c r="J295" s="8"/>
-      <c r="K295" s="8"/>
-      <c r="L295" s="8"/>
-      <c r="M295" s="8"/>
-      <c r="N295" s="8"/>
-      <c r="O295" s="8"/>
-      <c r="P295" s="8"/>
-      <c r="Q295" s="8"/>
-      <c r="R295" s="8"/>
-      <c r="S295" s="8"/>
-      <c r="T295" s="8"/>
-      <c r="U295" s="8"/>
-      <c r="V295" s="8"/>
-      <c r="W295" s="8"/>
-      <c r="X295" s="8"/>
-      <c r="Y295" s="8"/>
-      <c r="Z295" s="8"/>
-      <c r="AA295" s="8"/>
-      <c r="AB295" s="8"/>
-      <c r="AC295" s="8"/>
-      <c r="AD295" s="8"/>
-      <c r="AE295" s="8"/>
-      <c r="AF295" s="8"/>
-      <c r="AG295" s="8"/>
-      <c r="AH295" s="8"/>
-      <c r="AI295" s="8"/>
-      <c r="AJ295" s="8"/>
-      <c r="AK295" s="8"/>
-      <c r="AL295" s="8"/>
-      <c r="AM295" s="8"/>
-    </row>
-    <row r="296" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A296" s="8"/>
-      <c r="B296" s="8"/>
-      <c r="C296" s="8"/>
-      <c r="D296" s="8"/>
-      <c r="E296" s="8"/>
-      <c r="F296" s="8"/>
-      <c r="G296" s="8"/>
-      <c r="H296" s="8"/>
-      <c r="I296" s="8"/>
-      <c r="J296" s="8"/>
-      <c r="K296" s="8"/>
-      <c r="L296" s="8"/>
-      <c r="M296" s="8"/>
-      <c r="N296" s="8"/>
-      <c r="O296" s="8"/>
-      <c r="P296" s="8"/>
-      <c r="Q296" s="8"/>
-      <c r="R296" s="8"/>
-      <c r="S296" s="8"/>
-      <c r="T296" s="8"/>
-      <c r="U296" s="8"/>
-      <c r="V296" s="8"/>
-      <c r="W296" s="8"/>
-      <c r="X296" s="8"/>
-      <c r="Y296" s="8"/>
-      <c r="Z296" s="8"/>
-      <c r="AA296" s="8"/>
-      <c r="AB296" s="8"/>
-      <c r="AC296" s="8"/>
-      <c r="AD296" s="8"/>
-      <c r="AE296" s="8"/>
-      <c r="AF296" s="8"/>
-      <c r="AG296" s="8"/>
-      <c r="AH296" s="8"/>
-      <c r="AI296" s="8"/>
-      <c r="AJ296" s="8"/>
-      <c r="AK296" s="8"/>
-      <c r="AL296" s="8"/>
-      <c r="AM296" s="8"/>
-    </row>
-    <row r="297" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A297" s="8"/>
-      <c r="B297" s="8"/>
-      <c r="C297" s="8"/>
-      <c r="D297" s="8"/>
-      <c r="E297" s="8"/>
-      <c r="F297" s="8"/>
-      <c r="G297" s="8"/>
-      <c r="H297" s="8"/>
-      <c r="I297" s="8"/>
-      <c r="J297" s="8"/>
-      <c r="K297" s="8"/>
-      <c r="L297" s="8"/>
-      <c r="M297" s="8"/>
-      <c r="N297" s="8"/>
-      <c r="O297" s="8"/>
-      <c r="P297" s="8"/>
-      <c r="Q297" s="8"/>
-      <c r="R297" s="8"/>
-      <c r="S297" s="8"/>
-      <c r="T297" s="8"/>
-      <c r="U297" s="8"/>
-      <c r="V297" s="8"/>
-      <c r="W297" s="8"/>
-      <c r="X297" s="8"/>
-      <c r="Y297" s="8"/>
-      <c r="Z297" s="8"/>
-      <c r="AA297" s="8"/>
-      <c r="AB297" s="8"/>
-      <c r="AC297" s="8"/>
-      <c r="AD297" s="8"/>
-      <c r="AE297" s="8"/>
-      <c r="AF297" s="8"/>
-      <c r="AG297" s="8"/>
-      <c r="AH297" s="8"/>
-      <c r="AI297" s="8"/>
-      <c r="AJ297" s="8"/>
-      <c r="AK297" s="8"/>
-      <c r="AL297" s="8"/>
-      <c r="AM297" s="8"/>
-    </row>
-    <row r="298" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A298" s="8"/>
-      <c r="B298" s="8"/>
-      <c r="C298" s="8"/>
-      <c r="D298" s="8"/>
-      <c r="E298" s="8"/>
-      <c r="F298" s="8"/>
-      <c r="G298" s="8"/>
-      <c r="H298" s="8"/>
-      <c r="I298" s="8"/>
-      <c r="J298" s="8"/>
-      <c r="K298" s="8"/>
-      <c r="L298" s="8"/>
-      <c r="M298" s="8"/>
-      <c r="N298" s="8"/>
-      <c r="O298" s="8"/>
-      <c r="P298" s="8"/>
-      <c r="Q298" s="8"/>
-      <c r="R298" s="8"/>
-      <c r="S298" s="8"/>
-      <c r="T298" s="8"/>
-      <c r="U298" s="8"/>
-      <c r="V298" s="8"/>
-      <c r="W298" s="8"/>
-      <c r="X298" s="8"/>
-      <c r="Y298" s="8"/>
-      <c r="Z298" s="8"/>
-      <c r="AA298" s="8"/>
-      <c r="AB298" s="8"/>
-      <c r="AC298" s="8"/>
-      <c r="AD298" s="8"/>
-      <c r="AE298" s="8"/>
-      <c r="AF298" s="8"/>
-      <c r="AG298" s="8"/>
-      <c r="AH298" s="8"/>
-      <c r="AI298" s="8"/>
-      <c r="AJ298" s="8"/>
-      <c r="AK298" s="8"/>
-      <c r="AL298" s="8"/>
-      <c r="AM298" s="8"/>
-    </row>
-    <row r="299" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A299" s="8"/>
-      <c r="B299" s="8"/>
-      <c r="C299" s="8"/>
-      <c r="D299" s="8"/>
-      <c r="E299" s="8"/>
-      <c r="F299" s="8"/>
-      <c r="G299" s="8"/>
-      <c r="H299" s="8"/>
-      <c r="I299" s="8"/>
-      <c r="J299" s="8"/>
-      <c r="K299" s="8"/>
-      <c r="L299" s="8"/>
-      <c r="M299" s="8"/>
-      <c r="N299" s="8"/>
-      <c r="O299" s="8"/>
-      <c r="P299" s="8"/>
-      <c r="Q299" s="8"/>
-      <c r="R299" s="8"/>
-      <c r="S299" s="8"/>
-      <c r="T299" s="8"/>
-      <c r="U299" s="8"/>
-      <c r="V299" s="8"/>
-      <c r="W299" s="8"/>
-      <c r="X299" s="8"/>
-      <c r="Y299" s="8"/>
-      <c r="Z299" s="8"/>
-      <c r="AA299" s="8"/>
-      <c r="AB299" s="8"/>
-      <c r="AC299" s="8"/>
-      <c r="AD299" s="8"/>
-      <c r="AE299" s="8"/>
-      <c r="AF299" s="8"/>
-      <c r="AG299" s="8"/>
-      <c r="AH299" s="8"/>
-      <c r="AI299" s="8"/>
-      <c r="AJ299" s="8"/>
-      <c r="AK299" s="8"/>
-      <c r="AL299" s="8"/>
-      <c r="AM299" s="8"/>
-    </row>
-    <row r="300" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A300" s="8"/>
-      <c r="B300" s="8"/>
-      <c r="C300" s="8"/>
-      <c r="D300" s="8"/>
-      <c r="E300" s="8"/>
-      <c r="F300" s="8"/>
-      <c r="G300" s="8"/>
-      <c r="H300" s="8"/>
-      <c r="I300" s="8"/>
-      <c r="J300" s="8"/>
-      <c r="K300" s="8"/>
-      <c r="L300" s="8"/>
-      <c r="M300" s="8"/>
-      <c r="N300" s="8"/>
-      <c r="O300" s="8"/>
-      <c r="P300" s="8"/>
-      <c r="Q300" s="8"/>
-      <c r="R300" s="8"/>
-      <c r="S300" s="8"/>
-      <c r="T300" s="8"/>
-      <c r="U300" s="8"/>
-      <c r="V300" s="8"/>
-      <c r="W300" s="8"/>
-      <c r="X300" s="8"/>
-      <c r="Y300" s="8"/>
-      <c r="Z300" s="8"/>
-      <c r="AA300" s="8"/>
-      <c r="AB300" s="8"/>
-      <c r="AC300" s="8"/>
-      <c r="AD300" s="8"/>
-      <c r="AE300" s="8"/>
-      <c r="AF300" s="8"/>
-      <c r="AG300" s="8"/>
-      <c r="AH300" s="8"/>
-      <c r="AI300" s="8"/>
-      <c r="AJ300" s="8"/>
-      <c r="AK300" s="8"/>
-      <c r="AL300" s="8"/>
-      <c r="AM300" s="8"/>
-    </row>
-    <row r="301" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A301" s="8"/>
-      <c r="B301" s="8"/>
-      <c r="C301" s="8"/>
-      <c r="D301" s="8"/>
-      <c r="E301" s="8"/>
-      <c r="F301" s="8"/>
-      <c r="G301" s="8"/>
-      <c r="H301" s="8"/>
-      <c r="I301" s="8"/>
-      <c r="J301" s="8"/>
-      <c r="K301" s="8"/>
-      <c r="L301" s="8"/>
-      <c r="M301" s="8"/>
-      <c r="N301" s="8"/>
-      <c r="O301" s="8"/>
-      <c r="P301" s="8"/>
-      <c r="Q301" s="8"/>
-      <c r="R301" s="8"/>
-      <c r="S301" s="8"/>
-      <c r="T301" s="8"/>
-      <c r="U301" s="8"/>
-      <c r="V301" s="8"/>
-      <c r="W301" s="8"/>
-      <c r="X301" s="8"/>
-      <c r="Y301" s="8"/>
-      <c r="Z301" s="8"/>
-      <c r="AA301" s="8"/>
-      <c r="AB301" s="8"/>
-      <c r="AC301" s="8"/>
-      <c r="AD301" s="8"/>
-      <c r="AE301" s="8"/>
-      <c r="AF301" s="8"/>
-      <c r="AG301" s="8"/>
-      <c r="AH301" s="8"/>
-      <c r="AI301" s="8"/>
-      <c r="AJ301" s="8"/>
-      <c r="AK301" s="8"/>
-      <c r="AL301" s="8"/>
-      <c r="AM301" s="8"/>
-    </row>
-    <row r="302" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A302" s="8"/>
-      <c r="B302" s="8"/>
-      <c r="C302" s="8"/>
-      <c r="D302" s="8"/>
-      <c r="E302" s="8"/>
-      <c r="F302" s="8"/>
-      <c r="G302" s="8"/>
-      <c r="H302" s="8"/>
-      <c r="I302" s="8"/>
-      <c r="J302" s="8"/>
-      <c r="K302" s="8"/>
-      <c r="L302" s="8"/>
-      <c r="M302" s="8"/>
-      <c r="N302" s="8"/>
-      <c r="O302" s="8"/>
-      <c r="P302" s="8"/>
-      <c r="Q302" s="8"/>
-      <c r="R302" s="8"/>
-      <c r="S302" s="8"/>
-      <c r="T302" s="8"/>
-      <c r="U302" s="8"/>
-      <c r="V302" s="8"/>
-      <c r="W302" s="8"/>
-      <c r="X302" s="8"/>
-      <c r="Y302" s="8"/>
-      <c r="Z302" s="8"/>
-      <c r="AA302" s="8"/>
-      <c r="AB302" s="8"/>
-      <c r="AC302" s="8"/>
-      <c r="AD302" s="8"/>
-      <c r="AE302" s="8"/>
-      <c r="AF302" s="8"/>
-      <c r="AG302" s="8"/>
-      <c r="AH302" s="8"/>
-      <c r="AI302" s="8"/>
-      <c r="AJ302" s="8"/>
-      <c r="AK302" s="8"/>
-      <c r="AL302" s="8"/>
-      <c r="AM302" s="8"/>
-    </row>
-    <row r="303" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A303" s="8"/>
-      <c r="B303" s="8"/>
-      <c r="C303" s="8"/>
-      <c r="D303" s="8"/>
-      <c r="E303" s="8"/>
-      <c r="F303" s="8"/>
-      <c r="G303" s="8"/>
-      <c r="H303" s="8"/>
-      <c r="I303" s="8"/>
-      <c r="J303" s="8"/>
-      <c r="K303" s="8"/>
-      <c r="L303" s="8"/>
-      <c r="M303" s="8"/>
-      <c r="N303" s="8"/>
-      <c r="O303" s="8"/>
-      <c r="P303" s="8"/>
-      <c r="Q303" s="8"/>
-      <c r="R303" s="8"/>
-      <c r="S303" s="8"/>
-      <c r="T303" s="8"/>
-      <c r="U303" s="8"/>
-      <c r="V303" s="8"/>
-      <c r="W303" s="8"/>
-      <c r="X303" s="8"/>
-      <c r="Y303" s="8"/>
-      <c r="Z303" s="8"/>
-      <c r="AA303" s="8"/>
-      <c r="AB303" s="8"/>
-      <c r="AC303" s="8"/>
-      <c r="AD303" s="8"/>
-      <c r="AE303" s="8"/>
-      <c r="AF303" s="8"/>
-      <c r="AG303" s="8"/>
-      <c r="AH303" s="8"/>
-      <c r="AI303" s="8"/>
-      <c r="AJ303" s="8"/>
-      <c r="AK303" s="8"/>
-      <c r="AL303" s="8"/>
-      <c r="AM303" s="8"/>
-    </row>
-    <row r="304" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A304" s="8"/>
-      <c r="B304" s="8"/>
-      <c r="C304" s="8"/>
-      <c r="D304" s="8"/>
-      <c r="E304" s="8"/>
-      <c r="F304" s="8"/>
-      <c r="G304" s="8"/>
-      <c r="H304" s="8"/>
-      <c r="I304" s="8"/>
-      <c r="J304" s="8"/>
-      <c r="K304" s="8"/>
-      <c r="L304" s="8"/>
-      <c r="M304" s="8"/>
-      <c r="N304" s="8"/>
-      <c r="O304" s="8"/>
-      <c r="P304" s="8"/>
-      <c r="Q304" s="8"/>
-      <c r="R304" s="8"/>
-      <c r="S304" s="8"/>
-      <c r="T304" s="8"/>
-      <c r="U304" s="8"/>
-      <c r="V304" s="8"/>
-      <c r="W304" s="8"/>
-      <c r="X304" s="8"/>
-      <c r="Y304" s="8"/>
-      <c r="Z304" s="8"/>
-      <c r="AA304" s="8"/>
-      <c r="AB304" s="8"/>
-      <c r="AC304" s="8"/>
-      <c r="AD304" s="8"/>
-      <c r="AE304" s="8"/>
-      <c r="AF304" s="8"/>
-      <c r="AG304" s="8"/>
-      <c r="AH304" s="8"/>
-      <c r="AI304" s="8"/>
-      <c r="AJ304" s="8"/>
-      <c r="AK304" s="8"/>
-      <c r="AL304" s="8"/>
-      <c r="AM304" s="8"/>
-    </row>
-    <row r="305" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A305" s="8"/>
-      <c r="B305" s="8"/>
-      <c r="C305" s="8"/>
-      <c r="D305" s="8"/>
-      <c r="E305" s="8"/>
-      <c r="F305" s="8"/>
-      <c r="G305" s="8"/>
-      <c r="H305" s="8"/>
-      <c r="I305" s="8"/>
-      <c r="J305" s="8"/>
-      <c r="K305" s="8"/>
-      <c r="L305" s="8"/>
-      <c r="M305" s="8"/>
-      <c r="N305" s="8"/>
-      <c r="O305" s="8"/>
-      <c r="P305" s="8"/>
-      <c r="Q305" s="8"/>
-      <c r="R305" s="8"/>
-      <c r="S305" s="8"/>
-      <c r="T305" s="8"/>
-      <c r="U305" s="8"/>
-      <c r="V305" s="8"/>
-      <c r="W305" s="8"/>
-      <c r="X305" s="8"/>
-      <c r="Y305" s="8"/>
-      <c r="Z305" s="8"/>
-      <c r="AA305" s="8"/>
-      <c r="AB305" s="8"/>
-      <c r="AC305" s="8"/>
-      <c r="AD305" s="8"/>
-      <c r="AE305" s="8"/>
-      <c r="AF305" s="8"/>
-      <c r="AG305" s="8"/>
-      <c r="AH305" s="8"/>
-      <c r="AI305" s="8"/>
-      <c r="AJ305" s="8"/>
-      <c r="AK305" s="8"/>
-      <c r="AL305" s="8"/>
-      <c r="AM305" s="8"/>
-    </row>
   </sheetData>
-  <mergeCells count="101">
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="H5:K5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B17:E17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:E19"/>
-    <mergeCell ref="B21:E21"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="B10:E10"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
+  <mergeCells count="59">
+    <mergeCell ref="B44:F44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="B43:F43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="J40:K40"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="J38:K38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="J39:K39"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="J36:K36"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="J37:K37"/>
     <mergeCell ref="B34:F34"/>
     <mergeCell ref="H34:I34"/>
     <mergeCell ref="J34:K34"/>
@@ -30542,75 +29527,25 @@
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="H33:I33"/>
     <mergeCell ref="J33:K33"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J38:K38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="J36:K36"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="J37:K37"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="B43:F43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="J40:K40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="J41:K41"/>
-    <mergeCell ref="B46:F46"/>
-    <mergeCell ref="H46:I46"/>
-    <mergeCell ref="J46:K46"/>
-    <mergeCell ref="B47:F47"/>
-    <mergeCell ref="H47:I47"/>
-    <mergeCell ref="J47:K47"/>
-    <mergeCell ref="B44:F44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="B45:F45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="J45:K45"/>
-    <mergeCell ref="B50:F50"/>
-    <mergeCell ref="H50:I50"/>
-    <mergeCell ref="J50:K50"/>
-    <mergeCell ref="B51:F51"/>
-    <mergeCell ref="H51:I51"/>
-    <mergeCell ref="J51:K51"/>
-    <mergeCell ref="B48:F48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="J48:K48"/>
-    <mergeCell ref="B49:F49"/>
-    <mergeCell ref="H49:I49"/>
-    <mergeCell ref="J49:K49"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="H54:I54"/>
-    <mergeCell ref="J54:K54"/>
-    <mergeCell ref="B55:F55"/>
-    <mergeCell ref="H55:I55"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="B52:F52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="J52:K52"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="H53:I53"/>
-    <mergeCell ref="J53:K53"/>
-    <mergeCell ref="B58:F58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="J58:K58"/>
-    <mergeCell ref="B56:F56"/>
-    <mergeCell ref="H56:I56"/>
-    <mergeCell ref="J56:K56"/>
-    <mergeCell ref="B57:F57"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="J57:K57"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:E19"/>
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="H5:K5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B17:E17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>